<commit_message>
Now replaces values with constants in named references
</commit_message>
<xml_diff>
--- a/examples/utf8-strings.xlsx
+++ b/examples/utf8-strings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,10 +12,11 @@
     <sheet name="2015" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="named_area">工作表1!$A$2:$C$11</definedName>
     <definedName name="NetBalanceYear">'2015'!$B$3</definedName>
     <definedName name="Test.ii.test">工作表1!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -464,7 +465,7 @@
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Implemented the CHAR function in C and Ruby
</commit_message>
<xml_diff>
--- a/examples/utf8-strings.xlsx
+++ b/examples/utf8-strings.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>string</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Char</t>
+  </si>
+  <si>
+    <t>asfasd</t>
   </si>
 </sst>
 </file>
@@ -98,8 +101,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -119,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -127,6 +140,11 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -134,6 +152,11 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,10 +532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C270"/>
+  <dimension ref="A2:C276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C45" sqref="C15:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -579,2556 +602,2741 @@
         <f>CHAR(A15)</f>
         <v>_x0001_</v>
       </c>
+      <c r="C15">
+        <f t="shared" ref="C15:C45" si="0">LEN(B15)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <f t="shared" ref="A16:A79" si="0">A15+1</f>
+        <f t="shared" ref="A16:A79" si="1">A15+1</f>
         <v>2</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" ref="B16:B79" si="1">CHAR(A16)</f>
+        <f t="shared" ref="B16:B79" si="2">CHAR(A16)</f>
         <v>_x0002_</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0003_</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0003_</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0004_</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0004_</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0005_</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0005_</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0006_</v>
+      </c>
+      <c r="C20">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0006_</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0007_</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0007_</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0008_</v>
+      </c>
+      <c r="C22">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0008_</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">	</v>
+      </c>
+      <c r="C23">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">	</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 </v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000B_</v>
+      </c>
+      <c r="C25">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>_x000B_</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000C_</v>
+      </c>
+      <c r="C26">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>_x000C_</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000D_</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" si="1"/>
-        <v>_x000D_</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000E_</v>
+      </c>
+      <c r="C28">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="1"/>
-        <v>_x000E_</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000F_</v>
+      </c>
+      <c r="C29">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="1"/>
-        <v>_x000F_</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0010_</v>
+      </c>
+      <c r="C30">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0010_</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0011_</v>
+      </c>
+      <c r="C31">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0011_</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0012_</v>
+      </c>
+      <c r="C32">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0012_</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0013_</v>
+      </c>
+      <c r="C33">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0013_</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0014_</v>
+      </c>
+      <c r="C34">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0014_</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0015_</v>
+      </c>
+      <c r="C35">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0015_</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0016_</v>
+      </c>
+      <c r="C36">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0016_</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0017_</v>
+      </c>
+      <c r="C37">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B37" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0017_</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0018_</v>
+      </c>
+      <c r="C38">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0018_</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0019_</v>
+      </c>
+      <c r="C39">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="1"/>
-        <v>_x0019_</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001A_</v>
+      </c>
+      <c r="C40">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001A_</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001B_</v>
+      </c>
+      <c r="C41">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001B_</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001C_</v>
+      </c>
+      <c r="C42">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001C_</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001D_</v>
+      </c>
+      <c r="C43">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001D_</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001E_</v>
+      </c>
+      <c r="C44">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001E_</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001F_</v>
+      </c>
+      <c r="C45">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>_x001F_</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46">
+        <f>LEN(B46)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>!</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47">
+        <f>LEN(B47)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>$</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>%</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&amp;</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>)</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>*</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>+</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>.</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>/</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>:</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>;</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>=</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>?</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>@</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <f t="shared" ref="A80:A143" si="2">A79+1</f>
+        <f t="shared" ref="A80:A143" si="3">A79+1</f>
         <v>66</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" ref="B80:B143" si="3">CHAR(A80)</f>
+        <f t="shared" ref="B80:B143" si="4">CHAR(A80)</f>
         <v>B</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>G</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>H</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>I</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>J</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>K</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>L</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>O</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Q</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>R</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>U</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>V</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>X</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Y</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Z</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>\</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>^</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>_</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>`</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>a</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>b</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>c</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>d</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>e</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>f</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>g</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>h</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>i</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>j</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>k</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>l</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>m</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>n</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>o</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>p</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>q</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>r</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>s</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>t</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>u</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>v</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>w</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>x</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>y</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>z</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>{</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>|</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="B139" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>}</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="B140" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>~</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="B141" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v></v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="B142" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Ä</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="B143" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Å</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <f t="shared" ref="A144:A207" si="4">A143+1</f>
+        <f t="shared" ref="A144:A207" si="5">A143+1</f>
         <v>130</v>
       </c>
       <c r="B144" t="str">
-        <f t="shared" ref="B144:B207" si="5">CHAR(A144)</f>
+        <f t="shared" ref="B144:B207" si="6">CHAR(A144)</f>
         <v>Ç</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>131</v>
       </c>
       <c r="B145" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>É</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>132</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Ñ</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Ö</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Ü</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>á</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>à</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>â</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ä</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>139</v>
       </c>
       <c r="B153" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ã</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>å</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
       <c r="B155" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ç</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>142</v>
       </c>
       <c r="B156" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>é</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="B157" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>è</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="B158" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ê</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="B159" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ë</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="B160" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>í</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="B161" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ì</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="B162" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>î</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149</v>
       </c>
       <c r="B163" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ï</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="B164" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ñ</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="B165" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ó</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
       <c r="B166" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ò</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="B167" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ô</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="B168" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ö</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>õ</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ú</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ù</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>û</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ü</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>†</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="B175" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>°</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¢</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>£</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>§</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="B179" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>•</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="B180" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¶</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="B181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ß</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="B182" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>®</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="B183" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>©</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="B184" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>™</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>´</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¨</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>≠</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="B188" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Æ</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="B189" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Ø</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="B190" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>∞</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="B191" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>±</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="B192" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>≤</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
       <c r="B193" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>≥</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¥</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="B195" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>µ</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="B196" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>∂</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="B197" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>∑</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="B198" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>∏</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="B199" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>π</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="B200" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>∫</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="B201" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ª</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="B202" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>º</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="B203" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Ω</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="B204" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>æ</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="B205" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ø</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="B206" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¿</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>193</v>
       </c>
       <c r="B207" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>¡</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <f t="shared" ref="A208:A256" si="6">A207+1</f>
+        <f t="shared" ref="A208:A256" si="7">A207+1</f>
         <v>194</v>
       </c>
       <c r="B208" t="str">
-        <f t="shared" ref="B208:B271" si="7">CHAR(A208)</f>
+        <f t="shared" ref="B208:B271" si="8">CHAR(A208)</f>
         <v>¬</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>195</v>
       </c>
       <c r="B209" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>√</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>196</v>
       </c>
       <c r="B210" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ƒ</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>197</v>
       </c>
       <c r="B211" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>≈</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>198</v>
       </c>
       <c r="B212" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>∆</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>199</v>
       </c>
       <c r="B213" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>«</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="B214" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>»</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>201</v>
       </c>
       <c r="B215" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>…</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>202</v>
       </c>
       <c r="B216" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v> </v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>203</v>
       </c>
       <c r="B217" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>À</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>204</v>
       </c>
       <c r="B218" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ã</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>205</v>
       </c>
       <c r="B219" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Õ</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>206</v>
       </c>
       <c r="B220" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Œ</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>207</v>
       </c>
       <c r="B221" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>œ</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>208</v>
       </c>
       <c r="B222" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>–</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>209</v>
       </c>
       <c r="B223" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>—</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>210</v>
       </c>
       <c r="B224" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>“</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>211</v>
       </c>
       <c r="B225" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>”</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>212</v>
       </c>
       <c r="B226" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>‘</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>213</v>
       </c>
       <c r="B227" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>’</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>214</v>
       </c>
       <c r="B228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>÷</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>215</v>
       </c>
       <c r="B229" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>◊</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>216</v>
       </c>
       <c r="B230" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ÿ</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="B231" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ÿ</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>218</v>
       </c>
       <c r="B232" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>⁄</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>219</v>
       </c>
       <c r="B233" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>€</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>220</v>
       </c>
       <c r="B234" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>‹</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>221</v>
       </c>
       <c r="B235" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>›</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>222</v>
       </c>
       <c r="B236" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ﬁ</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>223</v>
       </c>
       <c r="B237" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ﬂ</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>224</v>
       </c>
       <c r="B238" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>‡</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>225</v>
       </c>
       <c r="B239" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>·</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>226</v>
       </c>
       <c r="B240" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>‚</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>227</v>
       </c>
       <c r="B241" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>„</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>228</v>
       </c>
       <c r="B242" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>‰</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>229</v>
       </c>
       <c r="B243" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Â</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>230</v>
       </c>
       <c r="B244" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ê</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>231</v>
       </c>
       <c r="B245" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Á</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>232</v>
       </c>
       <c r="B246" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ë</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>233</v>
       </c>
       <c r="B247" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>È</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>234</v>
       </c>
       <c r="B248" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Í</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>235</v>
       </c>
       <c r="B249" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Î</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>236</v>
       </c>
       <c r="B250" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ï</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>237</v>
       </c>
       <c r="B251" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ì</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>238</v>
       </c>
       <c r="B252" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ó</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>239</v>
       </c>
       <c r="B253" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ô</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="B254" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v></v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>241</v>
       </c>
       <c r="B255" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ò</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>242</v>
       </c>
       <c r="B256" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ú</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257">
-        <f t="shared" ref="A257:A268" si="8">A256+1</f>
+        <f t="shared" ref="A257:A268" si="9">A256+1</f>
         <v>243</v>
       </c>
       <c r="B257" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Û</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="B258" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Ù</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>245</v>
       </c>
       <c r="B259" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ı</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>246</v>
       </c>
       <c r="B260" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ˆ</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247</v>
       </c>
       <c r="B261" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˜</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248</v>
       </c>
       <c r="B262" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>¯</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249</v>
       </c>
       <c r="B263" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˘</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>250</v>
       </c>
       <c r="B264" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˙</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>251</v>
       </c>
       <c r="B265" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˚</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>252</v>
       </c>
       <c r="B266" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>¸</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>253</v>
       </c>
       <c r="B267" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˝</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>254</v>
       </c>
       <c r="B268" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>˛</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269">
-        <f t="shared" ref="A269" si="9">A268+1</f>
+        <f t="shared" ref="A269" si="10">A268+1</f>
         <v>255</v>
       </c>
       <c r="B269" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>ˇ</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270">
-        <f t="shared" ref="A270" si="10">A269+1</f>
+        <f t="shared" ref="A270" si="11">A269+1</f>
         <v>256</v>
       </c>
       <c r="B270" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="e">
+        <f>0/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B271" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="B272" t="e">
+        <f>CHAR(A272)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="str">
+        <f>"48"</f>
+        <v>48</v>
+      </c>
+      <c r="B273" t="str">
+        <f t="shared" ref="B273:B276" si="12">CHAR(A273)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>8</v>
+      </c>
+      <c r="B274" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275">
+        <v>-1</v>
+      </c>
+      <c r="B275" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276">
+        <v>97.12312</v>
+      </c>
+      <c r="B276" t="str">
+        <f t="shared" si="12"/>
+        <v>a</v>
       </c>
     </row>
   </sheetData>

</xml_diff>